<commit_message>
1k test pilot measurements
</commit_message>
<xml_diff>
--- a/RenderTimes.xlsx
+++ b/RenderTimes.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/573bcb74941738ce/Jonnas skit/Plugg/Exjobb/Kod/GitHub/BachelorDegreeProjectIT2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive\Jonnas skit\Plugg\Exjobb\Kod\GitHub\BachelorDegreeProjectIT2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F403D34-578A-4C29-8FF4-EE61CE159142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{0F403D34-578A-4C29-8FF4-EE61CE159142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7D63173-D763-463D-B509-5B3AFD2CBFDE}"/>
   <bookViews>
-    <workbookView xWindow="-18255" yWindow="630" windowWidth="17625" windowHeight="13020" xr2:uid="{AD91D73C-E77C-4A10-B30A-D46D165E264F}"/>
+    <workbookView xWindow="-18435" yWindow="405" windowWidth="17625" windowHeight="13020" xr2:uid="{AD91D73C-E77C-4A10-B30A-D46D165E264F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pilot" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +30,50 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>ApexCharts</t>
+  </si>
+  <si>
+    <t>Frappe Charts</t>
+  </si>
+  <si>
+    <t>Google Charts</t>
+  </si>
+  <si>
+    <t>TeeChart JS</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>One measurement per library only</t>
+  </si>
+  <si>
+    <t>Unit: ms, rounded to whole number</t>
+  </si>
+  <si>
+    <t>Bar charts only, settings barely touched</t>
+  </si>
+  <si>
+    <t>Shift+f5 done before each measurement to ignore cached content</t>
+  </si>
+  <si>
+    <t>Other browser windows and other applications are open - real test will be done on a separate machine</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -80,6 +124,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +427,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B9C930-3AFA-4D50-A31E-4E663B1C3175}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>